<commit_message>
[dataset-metrics-02][l]: metrics to determine what domains were scraped by Datopian EXCLUSIVELY and resources gathered and vice-versa
</commit_message>
<xml_diff>
--- a/tools/dataset_metrics/metrics.xlsx
+++ b/tools/dataset_metrics/metrics.xlsx
@@ -9,6 +9,8 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PAGE COUNT (DATOPIAN)" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PAGE COUNT (AIR)" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RESOURCE COUNT (DATOPIAN ONLY)" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RESOURCE COUNT (AIR ONLY)" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1153,4 +1155,266 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>resource count</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>stateaid.nysed.gov</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>data.nysed.gov</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>results.ed.gov</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>eric.ed.gov</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>p12.nysed.gov</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>emsc32.nysed.gov</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>pdp.ed.gov</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>americanenglish.state.gov</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>portal.nysed.gov</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ccsso.org</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>p1232.nysed.gov</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>resource count</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>fsadownload.ed.gov</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>fp.ed.gov</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>charterschoolcenter.ed.gov</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>y4y.ed.gov</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>surveys.ope.ed.gov</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>nslds.ed.gov</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>experimentalsites.ed.gov</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>nsldsfap.ed.gov</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ope.ed.gov</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>